<commit_message>
ACTUALIZA 2 OCT 2020
</commit_message>
<xml_diff>
--- a/CHILE/Agricultura/Emisiones CH4 Agricultura Chile 1990-2016.xlsx
+++ b/CHILE/Agricultura/Emisiones CH4 Agricultura Chile 1990-2016.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATAICC\CHILE\Agricultura\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-ICC\CHILE\Agricultura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C74A9B27-5365-4571-A9D8-75E553139062}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A83BA9A-D94D-42BC-9F5C-848E722A8D8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark1 (2)" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="20">
   <si>
     <t>Emisiones por Tipo de emisión</t>
   </si>
@@ -60,12 +61,33 @@
   <si>
     <t>Año</t>
   </si>
+  <si>
+    <t>Sector</t>
+  </si>
+  <si>
+    <t>Proceso</t>
+  </si>
+  <si>
+    <t>Agricultura</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>Emisiones (kton CH4)</t>
+  </si>
+  <si>
+    <t>Emisiones (kton CO2eq)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -215,8 +237,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,6 +424,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -557,7 +591,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -565,11 +599,15 @@
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -617,7 +655,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="31">
     <dxf>
       <font>
         <b/>
@@ -655,7 +693,307 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -897,6 +1235,45 @@
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -911,21 +1288,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="CH4_Agricultura_Chile" displayName="CH4_Agricultura_Chile" ref="A2:L29" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A2:L29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="CH4_Agricultura_Chile" displayName="CH4_Agricultura_Chile" ref="A2:L29" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+  <autoFilter ref="A2:L29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Año" dataDxfId="13"/>
-    <tableColumn id="2" name="3.A - Fermentación entérica" dataDxfId="12"/>
-    <tableColumn id="3" name="3.B - Gestión del estiércol" dataDxfId="11"/>
-    <tableColumn id="4" name="3.C - Cultivo del arroz" dataDxfId="10"/>
-    <tableColumn id="5" name="3.D - Suelos agrícolas" dataDxfId="9"/>
-    <tableColumn id="6" name="3.E - Quema prescrita de sabanas" dataDxfId="8"/>
-    <tableColumn id="7" name="3.F - Quema de residuos agrícola en el campo" dataDxfId="7"/>
-    <tableColumn id="8" name="3.G - Encalado" dataDxfId="6"/>
-    <tableColumn id="9" name="3.H - Aplicación de urea" dataDxfId="5"/>
-    <tableColumn id="10" name="3.I - Otros fertilizantes que contienen carbono" dataDxfId="4"/>
-    <tableColumn id="11" name="3.J - Otros" dataDxfId="3"/>
-    <tableColumn id="12" name="3 - Agricultura" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Año" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="3.A - Fermentación entérica" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="3.B - Gestión del estiércol" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="3.C - Cultivo del arroz" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="3.D - Suelos agrícolas" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="3.E - Quema prescrita de sabanas" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="3.F - Quema de residuos agrícola en el campo" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="3.G - Encalado" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="3.H - Aplicación de urea" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="3.I - Otros fertilizantes que contienen carbono" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="3.J - Otros" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="3 - Agricultura" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26EE8692-14F4-4147-880C-A7C7D7046398}" name="CH4_Agricultura_Chile3" displayName="CH4_Agricultura_Chile3" ref="A2:O56" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A2:O56" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{9DB7E131-B238-4B63-A460-0737A112B5CE}" name="Año" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{5134051A-AC8F-40F9-AA41-A67A3470425F}" name="Sector" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{D9A7E7FE-FD83-4C1C-8CE9-15500AA00804}" name="Proceso" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{C7876189-19B8-4537-A5F1-35458AF1D8FD}" name="Gas" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{16E5B5C6-A691-4C39-A384-E6CDA062423E}" name="Emisiones (kton CH4)" dataDxfId="13"/>
+    <tableColumn id="16" xr3:uid="{B4B99529-6663-4ABF-9EE9-931C2A936ACF}" name="Emisiones (kton CO2eq)" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{81D3779F-ED8D-41CF-8CA8-8E4539D7FA74}" name="3.C - Cultivo del arroz" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{BF1E4F70-0470-4E1F-B03D-471DD5C154E0}" name="3.D - Suelos agrícolas" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{1033F16B-216E-4554-9E60-98EED0C50E20}" name="3.E - Quema prescrita de sabanas" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{0486F489-C4F2-48D2-A3DC-71B0218381A8}" name="3.F - Quema de residuos agrícola en el campo" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{67C62C5A-94AD-4EF1-B4E4-B28C05CC6D6B}" name="3.G - Encalado" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{560CE1C4-F0C2-41A5-81F7-10C57555DE04}" name="3.H - Aplicación de urea" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{2CAED701-062C-41C8-B2B4-8C9D891E4E53}" name="3.I - Otros fertilizantes que contienen carbono" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{6936D843-9DDE-4C36-871F-ACABFA5074ED}" name="3.J - Otros" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{4A75532E-4316-4C8C-B0EC-A5AB2AC43D7D}" name="3 - Agricultura" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1227,46 +1628,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="38.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
     <col min="10" max="10" width="39" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1304,8 +1705,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1990</v>
       </c>
       <c r="B3" s="2">
@@ -1342,8 +1743,8 @@
         <v>284.0171398</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
         <v>1991</v>
       </c>
       <c r="B4" s="2">
@@ -1380,8 +1781,8 @@
         <v>287.11943689999998</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
         <v>1992</v>
       </c>
       <c r="B5" s="2">
@@ -1418,8 +1819,8 @@
         <v>295.02486900000002</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
         <v>1993</v>
       </c>
       <c r="B6" s="2">
@@ -1456,8 +1857,8 @@
         <v>304.34894750000001</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
         <v>1994</v>
       </c>
       <c r="B7" s="2">
@@ -1494,8 +1895,8 @@
         <v>314.7679852</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
         <v>1995</v>
       </c>
       <c r="B8" s="2">
@@ -1532,8 +1933,8 @@
         <v>320.5560792</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
         <v>1996</v>
       </c>
       <c r="B9" s="2">
@@ -1570,8 +1971,8 @@
         <v>322.893237</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
         <v>1997</v>
       </c>
       <c r="B10" s="2">
@@ -1608,8 +2009,8 @@
         <v>338.52818079999997</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>1998</v>
       </c>
       <c r="B11" s="2">
@@ -1646,8 +2047,8 @@
         <v>336.48648300000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
         <v>1999</v>
       </c>
       <c r="B12" s="2">
@@ -1684,8 +2085,8 @@
         <v>333.33398199999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>2000</v>
       </c>
       <c r="B13" s="2">
@@ -1722,8 +2123,8 @@
         <v>332.3534434</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
         <v>2001</v>
       </c>
       <c r="B14" s="2">
@@ -1760,8 +2161,8 @@
         <v>323.3759589</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <v>2002</v>
       </c>
       <c r="B15" s="2">
@@ -1798,8 +2199,8 @@
         <v>322.5217245</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <v>2003</v>
       </c>
       <c r="B16" s="2">
@@ -1836,8 +2237,8 @@
         <v>318.52107230000001</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <v>2004</v>
       </c>
       <c r="B17" s="2">
@@ -1874,8 +2275,8 @@
         <v>322.13517730000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
         <v>2005</v>
       </c>
       <c r="B18" s="2">
@@ -1912,8 +2313,8 @@
         <v>323.75195150000002</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
         <v>2006</v>
       </c>
       <c r="B19" s="2">
@@ -1950,8 +2351,8 @@
         <v>326.20438960000001</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
         <v>2007</v>
       </c>
       <c r="B20" s="2">
@@ -1988,8 +2389,8 @@
         <v>325.92189430000002</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
         <v>2008</v>
       </c>
       <c r="B21" s="2">
@@ -2026,8 +2427,8 @@
         <v>313.5969316</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
         <v>2009</v>
       </c>
       <c r="B22" s="2">
@@ -2064,8 +2465,8 @@
         <v>299.90997640000001</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
         <v>2010</v>
       </c>
       <c r="B23" s="2">
@@ -2102,8 +2503,8 @@
         <v>289.85902049999999</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
         <v>2011</v>
       </c>
       <c r="B24" s="2">
@@ -2140,8 +2541,8 @@
         <v>280.25508280000003</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
         <v>2012</v>
       </c>
       <c r="B25" s="2">
@@ -2178,8 +2579,8 @@
         <v>291.35017549999998</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
         <v>2013</v>
       </c>
       <c r="B26" s="2">
@@ -2216,8 +2617,8 @@
         <v>291.94883229999999</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
         <v>2014</v>
       </c>
       <c r="B27" s="2">
@@ -2254,8 +2655,8 @@
         <v>278.95255100000003</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
         <v>2015</v>
       </c>
       <c r="B28" s="2">
@@ -2292,8 +2693,8 @@
         <v>270.8206725</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
         <v>2016</v>
       </c>
       <c r="B29" s="2">
@@ -2340,4 +2741,2058 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9580AB30-9B6B-41AA-8F2C-047A57BE1050}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:O56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="38.109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="39" style="3" customWidth="1"/>
+    <col min="14" max="14" width="11" style="3" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.109375" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>1990</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
+        <v>219.54959930000001</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>6.5668850000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.5488267999999996</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>284.0171398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>1991</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>221.43015869999999</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>5.9946250000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>4.2799117999999998</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <v>287.11943689999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>1992</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>226.89692059999999</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>6.3996399999999998</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4.0877534000000004</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>295.02486900000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>1993</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2">
+        <v>234.77818790000001</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>5.8596199999999996</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>3.7077198</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>304.34894750000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>1994</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2">
+        <v>242.21451200000001</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>6.11754</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3.4327120999999998</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>314.7679852</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>1995</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2">
+        <v>245.61781149999999</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>6.8368950000000002</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>3.3736386999999999</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>320.5560792</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>1996</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2">
+        <v>245.78133159999999</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <v>6.4540449999999998</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3.0817393000000002</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>322.893237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>1997</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2">
+        <v>256.53864750000002</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>5.1910027000000003</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>3.1864675</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>338.52818079999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>1998</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2">
+        <v>254.57677279999999</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
+        <v>5.3804530000000002</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>3.1164743000000001</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0</v>
+      </c>
+      <c r="O11" s="2">
+        <v>336.48648300000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>1999</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2">
+        <v>252.21831449999999</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <v>2.9612440000000002</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2">
+        <v>2.5212994000000002</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0</v>
+      </c>
+      <c r="O12" s="2">
+        <v>333.33398199999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>2000</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <v>249.80261519999999</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <v>5.1922519999999999</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>2.5998698999999998</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>332.3534434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>2001</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2">
+        <v>249.53128380000001</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <v>5.7528249999999996</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>2.7012130000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <v>323.3759589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>2002</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2">
+        <v>247.3887512</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2">
+        <v>5.6379700000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>2.6209663000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0</v>
+      </c>
+      <c r="O15" s="2">
+        <v>322.5217245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>2003</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2">
+        <v>244.76677979999999</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2">
+        <v>5.688345</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2">
+        <v>2.5789493999999999</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0</v>
+      </c>
+      <c r="O16" s="2">
+        <v>318.52107230000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>2004</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>243.36327879999999</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2">
+        <v>5.0173500000000004</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2">
+        <v>2.4968995</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>322.13517730000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>2005</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>241.8287393</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2">
+        <v>5.0435449999999999</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2">
+        <v>2.2362962999999998</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0</v>
+      </c>
+      <c r="O18" s="2">
+        <v>323.75195150000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>2006</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2">
+        <v>240.6797718</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2">
+        <v>5.6379700000000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.9911418000000001</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0</v>
+      </c>
+      <c r="O19" s="2">
+        <v>326.20438960000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>2007</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="2">
+        <v>238.8738061</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2">
+        <v>4.3857280999999997</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1.4303273000000001</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2">
+        <v>0</v>
+      </c>
+      <c r="O20" s="2">
+        <v>325.92189430000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>2008</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2">
+        <v>229.61545620000001</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2">
+        <v>4.2234400000000001</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1.509471</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <v>313.5969316</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>2009</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="2">
+        <v>218.6590826</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2">
+        <v>4.7715199999999998</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.4276603000000001</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
+        <v>299.90997640000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="2">
+        <v>210.01662970000001</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2">
+        <v>4.9421904999999997</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.4760956000000001</v>
+      </c>
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>289.85902049999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>2011</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2">
+        <v>200.51033860000001</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2">
+        <v>5.0618815000000001</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.5492357999999999</v>
+      </c>
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2">
+        <v>0</v>
+      </c>
+      <c r="O24" s="2">
+        <v>280.25508280000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>2012</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="2">
+        <v>206.57436419999999</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2">
+        <v>4.8341865000000004</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1.3549028999999999</v>
+      </c>
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <v>0</v>
+      </c>
+      <c r="O25" s="2">
+        <v>291.35017549999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>2013</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2">
+        <v>211.6848541</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2">
+        <v>4.2314999999999996</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1.4342113000000001</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
+        <v>291.94883229999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>2014</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="2">
+        <v>202.5623397</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2">
+        <v>4.5131969999999999</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1.4055248</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <v>0</v>
+      </c>
+      <c r="O27" s="2">
+        <v>278.95255100000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="2">
+        <v>193.33985010000001</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2">
+        <v>4.7783709999999999</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1.5447434</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0</v>
+      </c>
+      <c r="N28" s="2">
+        <v>0</v>
+      </c>
+      <c r="O28" s="2">
+        <v>270.8206725</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="2">
+        <v>187.2807368</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2">
+        <v>5.34781</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1.0648981</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0</v>
+      </c>
+      <c r="N29" s="2">
+        <v>0</v>
+      </c>
+      <c r="O29" s="2">
+        <v>263.58165400000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>1990</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2">
+        <v>53.351828699999999</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>1991</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2">
+        <v>55.414741399999997</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>1992</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="2">
+        <v>57.640554999999999</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>1993</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2">
+        <v>60.003419800000003</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>1994</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="2">
+        <v>63.003221099999998</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>1995</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="2">
+        <v>64.727733999999998</v>
+      </c>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>1996</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="2">
+        <v>67.576121099999995</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>1997</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="2">
+        <v>73.6120631</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>1998</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="2">
+        <v>73.412782899999996</v>
+      </c>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>1999</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="2">
+        <v>75.633124100000003</v>
+      </c>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>2000</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="2">
+        <v>74.7587063</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>2001</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E41" s="2">
+        <v>65.390637100000006</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>2002</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="2">
+        <v>66.874037000000001</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>2003</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="2">
+        <v>65.486998099999994</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>2004</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="2">
+        <v>71.257649000000001</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>2005</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="2">
+        <v>74.643370899999994</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>2006</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="2">
+        <v>77.895505999999997</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>2007</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="2">
+        <v>81.232032799999999</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+      <c r="O47" s="2"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>2008</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" s="2">
+        <v>78.248564400000006</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A49" s="4">
+        <v>2009</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" s="2">
+        <v>75.051713500000005</v>
+      </c>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+      <c r="O49" s="2"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" s="4">
+        <v>2010</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="2">
+        <v>73.424104700000001</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" s="4">
+        <v>2011</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="2">
+        <v>73.133626899999996</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+      <c r="O51" s="2"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" s="4">
+        <v>2012</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="2">
+        <v>78.586721900000001</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="2"/>
+      <c r="N52" s="2"/>
+      <c r="O52" s="2"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" s="4">
+        <v>2013</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E53" s="2">
+        <v>74.598266899999999</v>
+      </c>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" s="4">
+        <v>2014</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="2">
+        <v>70.471489500000004</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+      <c r="O54" s="2"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55" s="4">
+        <v>2015</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="2">
+        <v>71.157708</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+      <c r="O55" s="2"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A56" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="2">
+        <v>69.888209099999997</v>
+      </c>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>